<commit_message>
Initial commit with project files
</commit_message>
<xml_diff>
--- a/Y2B_worklog_24-25_ADSAI (1).xlsx
+++ b/Y2B_worklog_24-25_ADSAI (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Desktop\Github_school\2025_B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73442629-9BB0-4983-A0B1-2B83E2CF5B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8C19B8-AD6B-40C3-BE27-83544C953796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30165" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="229">
   <si>
     <t>Date</t>
   </si>
@@ -829,6 +829,21 @@
   </si>
   <si>
     <t>Proceeded with gathering and organizing evidence.</t>
+  </si>
+  <si>
+    <t>ILO 1.6</t>
+  </si>
+  <si>
+    <t>ILO 5.1</t>
+  </si>
+  <si>
+    <t>ILO 8.6</t>
+  </si>
+  <si>
+    <t>ILO 8.7</t>
+  </si>
+  <si>
+    <t>ILO 2.6</t>
   </si>
 </sst>
 </file>
@@ -1331,6 +1346,26 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1347,8 +1382,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1366,24 +1399,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1505,10 +1520,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1815,8 +1826,8 @@
   <dimension ref="A1:K148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G124" sqref="G124"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E142" sqref="E142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
@@ -1869,53 +1880,53 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="71"/>
     </row>
     <row r="3" spans="1:11" ht="12.75">
       <c r="A3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="66"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="59"/>
     </row>
     <row r="4" spans="1:11" ht="27.75" customHeight="1">
       <c r="A4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="66"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="59"/>
     </row>
     <row r="5" spans="1:11" ht="12.75">
       <c r="A5" s="19">
@@ -1931,7 +1942,9 @@
         <v>69</v>
       </c>
       <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="F5" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="G5" s="22">
         <v>1.5</v>
       </c>
@@ -1961,7 +1974,9 @@
         <v>70</v>
       </c>
       <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="F6" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="G6" s="22">
         <v>1</v>
       </c>
@@ -1991,7 +2006,9 @@
         <v>71</v>
       </c>
       <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
+      <c r="F7" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="G7" s="22">
         <v>4</v>
       </c>
@@ -2021,7 +2038,9 @@
         <v>73</v>
       </c>
       <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
+      <c r="F8" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="G8" s="22">
         <v>2</v>
       </c>
@@ -2051,7 +2070,9 @@
         <v>71</v>
       </c>
       <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="F9" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="G9" s="22">
         <v>3</v>
       </c>
@@ -2081,7 +2102,9 @@
         <v>70</v>
       </c>
       <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="F10" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="G10" s="22">
         <v>1</v>
       </c>
@@ -2111,7 +2134,9 @@
         <v>71</v>
       </c>
       <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="F11" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="G11" s="22">
         <v>4</v>
       </c>
@@ -2141,7 +2166,9 @@
         <v>70</v>
       </c>
       <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
+      <c r="F12" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="G12" s="22">
         <v>1</v>
       </c>
@@ -2171,7 +2198,9 @@
         <v>72</v>
       </c>
       <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
+      <c r="F13" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="G13" s="22">
         <v>2</v>
       </c>
@@ -2201,7 +2230,9 @@
         <v>74</v>
       </c>
       <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
+      <c r="F14" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="G14" s="22">
         <v>2</v>
       </c>
@@ -2231,7 +2262,9 @@
         <v>71</v>
       </c>
       <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+      <c r="F15" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="G15" s="22">
         <v>2</v>
       </c>
@@ -2261,7 +2294,9 @@
         <v>70</v>
       </c>
       <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
+      <c r="F16" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="G16" s="22">
         <v>1</v>
       </c>
@@ -2291,7 +2326,9 @@
         <v>75</v>
       </c>
       <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
+      <c r="F17" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="G17" s="22">
         <v>1.5</v>
       </c>
@@ -2321,7 +2358,9 @@
         <v>76</v>
       </c>
       <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
+      <c r="F18" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="G18" s="22">
         <v>2</v>
       </c>
@@ -2351,7 +2390,9 @@
         <v>77</v>
       </c>
       <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
+      <c r="F19" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="G19" s="22">
         <v>3</v>
       </c>
@@ -2381,7 +2422,9 @@
         <v>70</v>
       </c>
       <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
+      <c r="F20" s="21" t="s">
+        <v>224</v>
+      </c>
       <c r="G20" s="22">
         <v>1</v>
       </c>
@@ -2422,53 +2465,53 @@
       <c r="K21" s="31"/>
     </row>
     <row r="22" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A22" s="67" t="s">
+      <c r="A22" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="62"/>
-      <c r="K22" s="63"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="71"/>
     </row>
     <row r="23" spans="1:11" ht="12.75">
       <c r="A23" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="66"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="59"/>
     </row>
     <row r="24" spans="1:11" ht="27.75" customHeight="1">
       <c r="A24" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="68" t="s">
+      <c r="B24" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="66"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="59"/>
     </row>
     <row r="25" spans="1:11" ht="12.75">
       <c r="A25" s="34">
@@ -2484,7 +2527,9 @@
         <v>78</v>
       </c>
       <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
+      <c r="F25" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G25" s="22">
         <v>0.5</v>
       </c>
@@ -2514,7 +2559,9 @@
         <v>79</v>
       </c>
       <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
+      <c r="F26" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G26" s="22">
         <v>2</v>
       </c>
@@ -2544,7 +2591,9 @@
         <v>70</v>
       </c>
       <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
+      <c r="F27" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G27" s="22">
         <v>1</v>
       </c>
@@ -2574,7 +2623,9 @@
         <v>80</v>
       </c>
       <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
+      <c r="F28" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G28" s="22">
         <v>3</v>
       </c>
@@ -2604,7 +2655,9 @@
         <v>81</v>
       </c>
       <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
+      <c r="F29" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G29" s="22">
         <v>2</v>
       </c>
@@ -2634,7 +2687,9 @@
         <v>70</v>
       </c>
       <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
+      <c r="F30" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G30" s="22">
         <v>0.5</v>
       </c>
@@ -2664,7 +2719,9 @@
         <v>82</v>
       </c>
       <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
+      <c r="F31" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G31" s="22">
         <v>2.5</v>
       </c>
@@ -2694,7 +2751,9 @@
         <v>83</v>
       </c>
       <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
+      <c r="F32" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G32" s="22">
         <v>2</v>
       </c>
@@ -2724,7 +2783,9 @@
         <v>70</v>
       </c>
       <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
+      <c r="F33" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G33" s="22">
         <v>1</v>
       </c>
@@ -2754,7 +2815,9 @@
         <v>84</v>
       </c>
       <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
+      <c r="F34" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G34" s="22">
         <v>3</v>
       </c>
@@ -2784,7 +2847,9 @@
         <v>85</v>
       </c>
       <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="F35" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G35" s="22">
         <v>2</v>
       </c>
@@ -2814,7 +2879,9 @@
         <v>70</v>
       </c>
       <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="F36" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G36" s="22">
         <v>1</v>
       </c>
@@ -2844,7 +2911,9 @@
         <v>86</v>
       </c>
       <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="F37" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G37" s="22">
         <v>2</v>
       </c>
@@ -2874,7 +2943,9 @@
         <v>86</v>
       </c>
       <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
+      <c r="F38" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G38" s="22">
         <v>3</v>
       </c>
@@ -2904,7 +2975,9 @@
         <v>87</v>
       </c>
       <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
+      <c r="F39" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G39" s="22">
         <v>2</v>
       </c>
@@ -2934,7 +3007,9 @@
         <v>70</v>
       </c>
       <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
+      <c r="F40" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G40" s="22">
         <v>1</v>
       </c>
@@ -2975,53 +3050,53 @@
       <c r="K41" s="31"/>
     </row>
     <row r="42" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A42" s="69" t="s">
+      <c r="A42" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="65"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="65"/>
-      <c r="J42" s="65"/>
-      <c r="K42" s="66"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="58"/>
+      <c r="J42" s="58"/>
+      <c r="K42" s="59"/>
     </row>
     <row r="43" spans="1:11" ht="12.75">
       <c r="A43" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="70" t="s">
+      <c r="B43" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="65"/>
-      <c r="D43" s="65"/>
-      <c r="E43" s="65"/>
-      <c r="F43" s="65"/>
-      <c r="G43" s="65"/>
-      <c r="H43" s="65"/>
-      <c r="I43" s="65"/>
-      <c r="J43" s="65"/>
-      <c r="K43" s="66"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="58"/>
+      <c r="J43" s="58"/>
+      <c r="K43" s="59"/>
     </row>
     <row r="44" spans="1:11" ht="27.75" customHeight="1">
       <c r="A44" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="70" t="s">
+      <c r="B44" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="65"/>
-      <c r="D44" s="65"/>
-      <c r="E44" s="65"/>
-      <c r="F44" s="65"/>
-      <c r="G44" s="65"/>
-      <c r="H44" s="65"/>
-      <c r="I44" s="65"/>
-      <c r="J44" s="65"/>
-      <c r="K44" s="66"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="58"/>
+      <c r="E44" s="58"/>
+      <c r="F44" s="58"/>
+      <c r="G44" s="58"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="58"/>
+      <c r="J44" s="58"/>
+      <c r="K44" s="59"/>
     </row>
     <row r="45" spans="1:11" ht="12.75">
       <c r="A45" s="19">
@@ -3037,7 +3112,9 @@
         <v>88</v>
       </c>
       <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
+      <c r="F45" s="21" t="s">
+        <v>226</v>
+      </c>
       <c r="G45" s="22">
         <v>2</v>
       </c>
@@ -3067,7 +3144,9 @@
         <v>70</v>
       </c>
       <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
+      <c r="F46" s="21" t="s">
+        <v>226</v>
+      </c>
       <c r="G46" s="22">
         <v>1</v>
       </c>
@@ -3097,7 +3176,9 @@
         <v>89</v>
       </c>
       <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
+      <c r="F47" s="21" t="s">
+        <v>226</v>
+      </c>
       <c r="G47" s="22">
         <v>3</v>
       </c>
@@ -3127,7 +3208,9 @@
         <v>90</v>
       </c>
       <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
+      <c r="F48" s="21" t="s">
+        <v>226</v>
+      </c>
       <c r="G48" s="22">
         <v>3</v>
       </c>
@@ -3157,7 +3240,9 @@
         <v>70</v>
       </c>
       <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
+      <c r="F49" s="21" t="s">
+        <v>226</v>
+      </c>
       <c r="G49" s="22">
         <v>1</v>
       </c>
@@ -3187,7 +3272,9 @@
         <v>92</v>
       </c>
       <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
+      <c r="F50" s="21" t="s">
+        <v>226</v>
+      </c>
       <c r="G50" s="22">
         <v>3</v>
       </c>
@@ -3217,7 +3304,9 @@
         <v>93</v>
       </c>
       <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
+      <c r="F51" s="21" t="s">
+        <v>226</v>
+      </c>
       <c r="G51" s="22">
         <v>0.5</v>
       </c>
@@ -3247,7 +3336,9 @@
         <v>94</v>
       </c>
       <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
+      <c r="F52" s="21" t="s">
+        <v>226</v>
+      </c>
       <c r="G52" s="22">
         <v>0.5</v>
       </c>
@@ -3277,7 +3368,9 @@
         <v>95</v>
       </c>
       <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
+      <c r="F53" s="21" t="s">
+        <v>226</v>
+      </c>
       <c r="G53" s="22">
         <v>4</v>
       </c>
@@ -3307,7 +3400,9 @@
         <v>91</v>
       </c>
       <c r="E54" s="21"/>
-      <c r="F54" s="21"/>
+      <c r="F54" s="21" t="s">
+        <v>226</v>
+      </c>
       <c r="G54" s="22">
         <v>3</v>
       </c>
@@ -3337,7 +3432,9 @@
         <v>96</v>
       </c>
       <c r="E55" s="21"/>
-      <c r="F55" s="21"/>
+      <c r="F55" s="21" t="s">
+        <v>226</v>
+      </c>
       <c r="G55" s="22">
         <v>1</v>
       </c>
@@ -3367,7 +3464,9 @@
         <v>95</v>
       </c>
       <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
+      <c r="F56" s="21" t="s">
+        <v>226</v>
+      </c>
       <c r="G56" s="22">
         <v>3</v>
       </c>
@@ -3397,7 +3496,9 @@
         <v>97</v>
       </c>
       <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
+      <c r="F57" s="21" t="s">
+        <v>226</v>
+      </c>
       <c r="G57" s="22">
         <v>2</v>
       </c>
@@ -3427,7 +3528,9 @@
         <v>70</v>
       </c>
       <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
+      <c r="F58" s="21" t="s">
+        <v>226</v>
+      </c>
       <c r="G58" s="22">
         <v>1</v>
       </c>
@@ -3457,7 +3560,9 @@
         <v>98</v>
       </c>
       <c r="E59" s="21"/>
-      <c r="F59" s="21"/>
+      <c r="F59" s="21" t="s">
+        <v>226</v>
+      </c>
       <c r="G59" s="22">
         <v>1</v>
       </c>
@@ -3498,53 +3603,53 @@
       <c r="K60" s="31"/>
     </row>
     <row r="61" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A61" s="71" t="s">
+      <c r="A61" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="B61" s="65"/>
-      <c r="C61" s="65"/>
-      <c r="D61" s="65"/>
-      <c r="E61" s="65"/>
-      <c r="F61" s="65"/>
-      <c r="G61" s="65"/>
-      <c r="H61" s="65"/>
-      <c r="I61" s="65"/>
-      <c r="J61" s="65"/>
-      <c r="K61" s="66"/>
+      <c r="B61" s="58"/>
+      <c r="C61" s="58"/>
+      <c r="D61" s="58"/>
+      <c r="E61" s="58"/>
+      <c r="F61" s="58"/>
+      <c r="G61" s="58"/>
+      <c r="H61" s="58"/>
+      <c r="I61" s="58"/>
+      <c r="J61" s="58"/>
+      <c r="K61" s="59"/>
     </row>
     <row r="62" spans="1:11" ht="12.75">
       <c r="A62" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B62" s="73" t="s">
+      <c r="B62" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="C62" s="65"/>
-      <c r="D62" s="65"/>
-      <c r="E62" s="65"/>
-      <c r="F62" s="65"/>
-      <c r="G62" s="65"/>
-      <c r="H62" s="65"/>
-      <c r="I62" s="65"/>
-      <c r="J62" s="65"/>
-      <c r="K62" s="66"/>
+      <c r="C62" s="58"/>
+      <c r="D62" s="58"/>
+      <c r="E62" s="58"/>
+      <c r="F62" s="58"/>
+      <c r="G62" s="58"/>
+      <c r="H62" s="58"/>
+      <c r="I62" s="58"/>
+      <c r="J62" s="58"/>
+      <c r="K62" s="59"/>
     </row>
     <row r="63" spans="1:11" ht="27.75" customHeight="1">
       <c r="A63" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B63" s="73" t="s">
+      <c r="B63" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="C63" s="65"/>
-      <c r="D63" s="65"/>
-      <c r="E63" s="65"/>
-      <c r="F63" s="65"/>
-      <c r="G63" s="65"/>
-      <c r="H63" s="65"/>
-      <c r="I63" s="65"/>
-      <c r="J63" s="65"/>
-      <c r="K63" s="66"/>
+      <c r="C63" s="58"/>
+      <c r="D63" s="58"/>
+      <c r="E63" s="58"/>
+      <c r="F63" s="58"/>
+      <c r="G63" s="58"/>
+      <c r="H63" s="58"/>
+      <c r="I63" s="58"/>
+      <c r="J63" s="58"/>
+      <c r="K63" s="59"/>
     </row>
     <row r="64" spans="1:11" ht="12.75">
       <c r="A64" s="19">
@@ -3560,7 +3665,9 @@
         <v>155</v>
       </c>
       <c r="E64" s="21"/>
-      <c r="F64" s="21"/>
+      <c r="F64" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="G64" s="22">
         <v>3</v>
       </c>
@@ -3590,7 +3697,9 @@
         <v>70</v>
       </c>
       <c r="E65" s="21"/>
-      <c r="F65" s="21"/>
+      <c r="F65" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="G65" s="22">
         <v>1</v>
       </c>
@@ -3620,7 +3729,9 @@
         <v>99</v>
       </c>
       <c r="E66" s="21"/>
-      <c r="F66" s="21"/>
+      <c r="F66" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="G66" s="22">
         <v>2</v>
       </c>
@@ -3650,7 +3761,9 @@
         <v>100</v>
       </c>
       <c r="E67" s="21"/>
-      <c r="F67" s="21"/>
+      <c r="F67" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="G67" s="22">
         <v>3</v>
       </c>
@@ -3680,7 +3793,9 @@
         <v>70</v>
       </c>
       <c r="E68" s="21"/>
-      <c r="F68" s="21"/>
+      <c r="F68" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="G68" s="22">
         <v>1</v>
       </c>
@@ -3710,7 +3825,9 @@
         <v>101</v>
       </c>
       <c r="E69" s="21"/>
-      <c r="F69" s="21"/>
+      <c r="F69" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="G69" s="22">
         <v>2</v>
       </c>
@@ -3740,7 +3857,9 @@
         <v>102</v>
       </c>
       <c r="E70" s="21"/>
-      <c r="F70" s="21"/>
+      <c r="F70" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="G70" s="22">
         <v>4</v>
       </c>
@@ -3770,7 +3889,9 @@
         <v>70</v>
       </c>
       <c r="E71" s="21"/>
-      <c r="F71" s="21"/>
+      <c r="F71" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="G71" s="22">
         <v>1</v>
       </c>
@@ -3800,7 +3921,9 @@
         <v>103</v>
       </c>
       <c r="E72" s="21"/>
-      <c r="F72" s="21"/>
+      <c r="F72" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="G72" s="22">
         <v>2</v>
       </c>
@@ -3830,7 +3953,9 @@
         <v>104</v>
       </c>
       <c r="E73" s="21"/>
-      <c r="F73" s="21"/>
+      <c r="F73" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="G73" s="22">
         <v>3</v>
       </c>
@@ -3860,7 +3985,9 @@
         <v>105</v>
       </c>
       <c r="E74" s="21"/>
-      <c r="F74" s="21"/>
+      <c r="F74" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="G74" s="22">
         <v>4</v>
       </c>
@@ -3890,7 +4017,9 @@
         <v>70</v>
       </c>
       <c r="E75" s="21"/>
-      <c r="F75" s="21"/>
+      <c r="F75" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="G75" s="22">
         <v>1</v>
       </c>
@@ -3920,7 +4049,9 @@
         <v>105</v>
       </c>
       <c r="E76" s="21"/>
-      <c r="F76" s="21"/>
+      <c r="F76" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="G76" s="22">
         <v>1</v>
       </c>
@@ -3950,7 +4081,9 @@
         <v>106</v>
       </c>
       <c r="E77" s="21"/>
-      <c r="F77" s="21"/>
+      <c r="F77" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="G77" s="22">
         <v>4</v>
       </c>
@@ -3980,7 +4113,9 @@
         <v>70</v>
       </c>
       <c r="E78" s="21"/>
-      <c r="F78" s="21"/>
+      <c r="F78" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="G78" s="22">
         <v>1</v>
       </c>
@@ -4010,7 +4145,9 @@
         <v>106</v>
       </c>
       <c r="E79" s="21"/>
-      <c r="F79" s="21"/>
+      <c r="F79" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="G79" s="22">
         <v>1</v>
       </c>
@@ -4051,53 +4188,53 @@
       <c r="K80" s="31"/>
     </row>
     <row r="81" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A81" s="76" t="s">
+      <c r="A81" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="B81" s="65"/>
-      <c r="C81" s="65"/>
-      <c r="D81" s="65"/>
-      <c r="E81" s="65"/>
-      <c r="F81" s="65"/>
-      <c r="G81" s="65"/>
-      <c r="H81" s="65"/>
-      <c r="I81" s="65"/>
-      <c r="J81" s="65"/>
-      <c r="K81" s="66"/>
+      <c r="B81" s="58"/>
+      <c r="C81" s="58"/>
+      <c r="D81" s="58"/>
+      <c r="E81" s="58"/>
+      <c r="F81" s="58"/>
+      <c r="G81" s="58"/>
+      <c r="H81" s="58"/>
+      <c r="I81" s="58"/>
+      <c r="J81" s="58"/>
+      <c r="K81" s="59"/>
     </row>
     <row r="82" spans="1:11" ht="12.75">
       <c r="A82" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B82" s="77" t="s">
-        <v>54</v>
-      </c>
-      <c r="C82" s="65"/>
-      <c r="D82" s="65"/>
-      <c r="E82" s="65"/>
-      <c r="F82" s="65"/>
-      <c r="G82" s="65"/>
-      <c r="H82" s="65"/>
-      <c r="I82" s="65"/>
-      <c r="J82" s="65"/>
-      <c r="K82" s="66"/>
+      <c r="B82" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="C82" s="58"/>
+      <c r="D82" s="58"/>
+      <c r="E82" s="58"/>
+      <c r="F82" s="58"/>
+      <c r="G82" s="58"/>
+      <c r="H82" s="58"/>
+      <c r="I82" s="58"/>
+      <c r="J82" s="58"/>
+      <c r="K82" s="59"/>
     </row>
     <row r="83" spans="1:11" ht="27.75" customHeight="1">
       <c r="A83" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B83" s="77" t="s">
+      <c r="B83" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="C83" s="65"/>
-      <c r="D83" s="65"/>
-      <c r="E83" s="65"/>
-      <c r="F83" s="65"/>
-      <c r="G83" s="65"/>
-      <c r="H83" s="65"/>
-      <c r="I83" s="65"/>
-      <c r="J83" s="65"/>
-      <c r="K83" s="66"/>
+      <c r="C83" s="58"/>
+      <c r="D83" s="58"/>
+      <c r="E83" s="58"/>
+      <c r="F83" s="58"/>
+      <c r="G83" s="58"/>
+      <c r="H83" s="58"/>
+      <c r="I83" s="58"/>
+      <c r="J83" s="58"/>
+      <c r="K83" s="59"/>
     </row>
     <row r="84" spans="1:11" ht="12.75">
       <c r="A84" s="19">
@@ -4113,7 +4250,9 @@
         <v>107</v>
       </c>
       <c r="E84" s="21"/>
-      <c r="F84" s="21"/>
+      <c r="F84" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G84" s="22">
         <v>2</v>
       </c>
@@ -4143,7 +4282,9 @@
         <v>70</v>
       </c>
       <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
+      <c r="F85" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G85" s="22">
         <v>1</v>
       </c>
@@ -4173,7 +4314,9 @@
         <v>108</v>
       </c>
       <c r="E86" s="21"/>
-      <c r="F86" s="21"/>
+      <c r="F86" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G86" s="22">
         <v>4</v>
       </c>
@@ -4203,7 +4346,9 @@
         <v>70</v>
       </c>
       <c r="E87" s="21"/>
-      <c r="F87" s="21"/>
+      <c r="F87" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G87" s="22">
         <v>0.5</v>
       </c>
@@ -4233,7 +4378,9 @@
         <v>109</v>
       </c>
       <c r="E88" s="21"/>
-      <c r="F88" s="21"/>
+      <c r="F88" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G88" s="22">
         <v>2</v>
       </c>
@@ -4263,7 +4410,9 @@
         <v>70</v>
       </c>
       <c r="E89" s="21"/>
-      <c r="F89" s="21"/>
+      <c r="F89" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G89" s="22">
         <v>1</v>
       </c>
@@ -4293,7 +4442,9 @@
         <v>110</v>
       </c>
       <c r="E90" s="21"/>
-      <c r="F90" s="21"/>
+      <c r="F90" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G90" s="22">
         <v>2</v>
       </c>
@@ -4323,7 +4474,9 @@
         <v>111</v>
       </c>
       <c r="E91" s="21"/>
-      <c r="F91" s="21"/>
+      <c r="F91" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G91" s="22">
         <v>3</v>
       </c>
@@ -4353,7 +4506,9 @@
         <v>70</v>
       </c>
       <c r="E92" s="21"/>
-      <c r="F92" s="21"/>
+      <c r="F92" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G92" s="22">
         <v>1</v>
       </c>
@@ -4383,7 +4538,9 @@
         <v>112</v>
       </c>
       <c r="E93" s="21"/>
-      <c r="F93" s="21"/>
+      <c r="F93" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G93" s="22">
         <v>2</v>
       </c>
@@ -4413,7 +4570,9 @@
         <v>113</v>
       </c>
       <c r="E94" s="21"/>
-      <c r="F94" s="21"/>
+      <c r="F94" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G94" s="22">
         <v>3</v>
       </c>
@@ -4443,7 +4602,9 @@
         <v>114</v>
       </c>
       <c r="E95" s="21"/>
-      <c r="F95" s="21"/>
+      <c r="F95" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G95" s="22">
         <v>4</v>
       </c>
@@ -4473,7 +4634,9 @@
         <v>70</v>
       </c>
       <c r="E96" s="21"/>
-      <c r="F96" s="21"/>
+      <c r="F96" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G96" s="22">
         <v>1</v>
       </c>
@@ -4503,7 +4666,9 @@
         <v>114</v>
       </c>
       <c r="E97" s="21"/>
-      <c r="F97" s="21"/>
+      <c r="F97" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G97" s="22">
         <v>4</v>
       </c>
@@ -4533,7 +4698,9 @@
         <v>70</v>
       </c>
       <c r="E98" s="21"/>
-      <c r="F98" s="21"/>
+      <c r="F98" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G98" s="22">
         <v>1</v>
       </c>
@@ -4574,53 +4741,53 @@
       <c r="K99" s="31"/>
     </row>
     <row r="100" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A100" s="78" t="s">
+      <c r="A100" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="B100" s="65"/>
-      <c r="C100" s="65"/>
-      <c r="D100" s="65"/>
-      <c r="E100" s="65"/>
-      <c r="F100" s="65"/>
-      <c r="G100" s="65"/>
-      <c r="H100" s="65"/>
-      <c r="I100" s="65"/>
-      <c r="J100" s="65"/>
-      <c r="K100" s="66"/>
+      <c r="B100" s="58"/>
+      <c r="C100" s="58"/>
+      <c r="D100" s="58"/>
+      <c r="E100" s="58"/>
+      <c r="F100" s="58"/>
+      <c r="G100" s="58"/>
+      <c r="H100" s="58"/>
+      <c r="I100" s="58"/>
+      <c r="J100" s="58"/>
+      <c r="K100" s="59"/>
     </row>
     <row r="101" spans="1:11" ht="12.75">
       <c r="A101" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="B101" s="74" t="s">
+      <c r="B101" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C101" s="65"/>
-      <c r="D101" s="65"/>
-      <c r="E101" s="65"/>
-      <c r="F101" s="65"/>
-      <c r="G101" s="65"/>
-      <c r="H101" s="65"/>
-      <c r="I101" s="65"/>
-      <c r="J101" s="65"/>
-      <c r="K101" s="66"/>
+      <c r="C101" s="58"/>
+      <c r="D101" s="58"/>
+      <c r="E101" s="58"/>
+      <c r="F101" s="58"/>
+      <c r="G101" s="58"/>
+      <c r="H101" s="58"/>
+      <c r="I101" s="58"/>
+      <c r="J101" s="58"/>
+      <c r="K101" s="59"/>
     </row>
     <row r="102" spans="1:11" ht="27.75" customHeight="1">
       <c r="A102" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B102" s="74" t="s">
+      <c r="B102" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C102" s="65"/>
-      <c r="D102" s="65"/>
-      <c r="E102" s="65"/>
-      <c r="F102" s="65"/>
-      <c r="G102" s="65"/>
-      <c r="H102" s="65"/>
-      <c r="I102" s="65"/>
-      <c r="J102" s="65"/>
-      <c r="K102" s="66"/>
+      <c r="C102" s="58"/>
+      <c r="D102" s="58"/>
+      <c r="E102" s="58"/>
+      <c r="F102" s="58"/>
+      <c r="G102" s="58"/>
+      <c r="H102" s="58"/>
+      <c r="I102" s="58"/>
+      <c r="J102" s="58"/>
+      <c r="K102" s="59"/>
     </row>
     <row r="103" spans="1:11" ht="12.75">
       <c r="A103" s="19">
@@ -4636,7 +4803,9 @@
         <v>115</v>
       </c>
       <c r="E103" s="21"/>
-      <c r="F103" s="21"/>
+      <c r="F103" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G103" s="22">
         <v>0</v>
       </c>
@@ -4666,7 +4835,9 @@
         <v>115</v>
       </c>
       <c r="E104" s="21"/>
-      <c r="F104" s="21"/>
+      <c r="F104" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G104" s="22">
         <v>0</v>
       </c>
@@ -4696,7 +4867,9 @@
         <v>114</v>
       </c>
       <c r="E105" s="21"/>
-      <c r="F105" s="21"/>
+      <c r="F105" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G105" s="22">
         <v>4</v>
       </c>
@@ -4726,7 +4899,9 @@
         <v>70</v>
       </c>
       <c r="E106" s="21"/>
-      <c r="F106" s="21"/>
+      <c r="F106" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G106" s="22">
         <v>1</v>
       </c>
@@ -4756,7 +4931,9 @@
         <v>177</v>
       </c>
       <c r="E107" s="21"/>
-      <c r="F107" s="21"/>
+      <c r="F107" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G107" s="22">
         <v>3</v>
       </c>
@@ -4786,7 +4963,9 @@
         <v>116</v>
       </c>
       <c r="E108" s="21"/>
-      <c r="F108" s="21"/>
+      <c r="F108" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G108" s="22">
         <v>4</v>
       </c>
@@ -4816,7 +4995,9 @@
         <v>70</v>
       </c>
       <c r="E109" s="21"/>
-      <c r="F109" s="21"/>
+      <c r="F109" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G109" s="22">
         <v>1</v>
       </c>
@@ -4846,7 +5027,9 @@
         <v>117</v>
       </c>
       <c r="E110" s="21"/>
-      <c r="F110" s="21"/>
+      <c r="F110" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G110" s="22">
         <v>2</v>
       </c>
@@ -4876,7 +5059,9 @@
         <v>118</v>
       </c>
       <c r="E111" s="21"/>
-      <c r="F111" s="21"/>
+      <c r="F111" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G111" s="22">
         <v>1</v>
       </c>
@@ -4906,7 +5091,9 @@
         <v>70</v>
       </c>
       <c r="E112" s="21"/>
-      <c r="F112" s="21"/>
+      <c r="F112" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G112" s="22">
         <v>1</v>
       </c>
@@ -4936,7 +5123,9 @@
         <v>119</v>
       </c>
       <c r="E113" s="21"/>
-      <c r="F113" s="21"/>
+      <c r="F113" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G113" s="22">
         <v>4</v>
       </c>
@@ -4966,7 +5155,9 @@
         <v>120</v>
       </c>
       <c r="E114" s="21"/>
-      <c r="F114" s="21"/>
+      <c r="F114" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G114" s="22">
         <v>4</v>
       </c>
@@ -4996,7 +5187,9 @@
         <v>176</v>
       </c>
       <c r="E115" s="21"/>
-      <c r="F115" s="21"/>
+      <c r="F115" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G115" s="22">
         <v>1</v>
       </c>
@@ -5026,7 +5219,9 @@
         <v>176</v>
       </c>
       <c r="E116" s="21"/>
-      <c r="F116" s="21"/>
+      <c r="F116" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G116" s="22">
         <v>4</v>
       </c>
@@ -5056,7 +5251,9 @@
         <v>192</v>
       </c>
       <c r="E117" s="21"/>
-      <c r="F117" s="21"/>
+      <c r="F117" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G117" s="22">
         <v>4</v>
       </c>
@@ -5097,53 +5294,53 @@
       <c r="K118" s="31"/>
     </row>
     <row r="119" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A119" s="75" t="s">
+      <c r="A119" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="B119" s="65"/>
-      <c r="C119" s="65"/>
-      <c r="D119" s="65"/>
-      <c r="E119" s="65"/>
-      <c r="F119" s="65"/>
-      <c r="G119" s="65"/>
-      <c r="H119" s="65"/>
-      <c r="I119" s="65"/>
-      <c r="J119" s="65"/>
-      <c r="K119" s="66"/>
+      <c r="B119" s="58"/>
+      <c r="C119" s="58"/>
+      <c r="D119" s="58"/>
+      <c r="E119" s="58"/>
+      <c r="F119" s="58"/>
+      <c r="G119" s="58"/>
+      <c r="H119" s="58"/>
+      <c r="I119" s="58"/>
+      <c r="J119" s="58"/>
+      <c r="K119" s="59"/>
     </row>
     <row r="120" spans="1:11" ht="12.75">
       <c r="A120" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B120" s="72" t="s">
+      <c r="B120" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="C120" s="65"/>
-      <c r="D120" s="65"/>
-      <c r="E120" s="65"/>
-      <c r="F120" s="65"/>
-      <c r="G120" s="65"/>
-      <c r="H120" s="65"/>
-      <c r="I120" s="65"/>
-      <c r="J120" s="65"/>
-      <c r="K120" s="66"/>
+      <c r="C120" s="58"/>
+      <c r="D120" s="58"/>
+      <c r="E120" s="58"/>
+      <c r="F120" s="58"/>
+      <c r="G120" s="58"/>
+      <c r="H120" s="58"/>
+      <c r="I120" s="58"/>
+      <c r="J120" s="58"/>
+      <c r="K120" s="59"/>
     </row>
     <row r="121" spans="1:11" ht="28.5" customHeight="1">
       <c r="A121" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B121" s="72" t="s">
+      <c r="B121" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C121" s="65"/>
-      <c r="D121" s="65"/>
-      <c r="E121" s="65"/>
-      <c r="F121" s="65"/>
-      <c r="G121" s="65"/>
-      <c r="H121" s="65"/>
-      <c r="I121" s="65"/>
-      <c r="J121" s="65"/>
-      <c r="K121" s="66"/>
+      <c r="C121" s="58"/>
+      <c r="D121" s="58"/>
+      <c r="E121" s="58"/>
+      <c r="F121" s="58"/>
+      <c r="G121" s="58"/>
+      <c r="H121" s="58"/>
+      <c r="I121" s="58"/>
+      <c r="J121" s="58"/>
+      <c r="K121" s="59"/>
     </row>
     <row r="122" spans="1:11" ht="12.75">
       <c r="A122" s="19">
@@ -5159,7 +5356,9 @@
         <v>188</v>
       </c>
       <c r="E122" s="21"/>
-      <c r="F122" s="21"/>
+      <c r="F122" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G122" s="22">
         <v>3</v>
       </c>
@@ -5189,7 +5388,9 @@
         <v>189</v>
       </c>
       <c r="E123" s="21"/>
-      <c r="F123" s="21"/>
+      <c r="F123" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G123" s="22">
         <v>3</v>
       </c>
@@ -5219,7 +5420,9 @@
         <v>189</v>
       </c>
       <c r="E124" s="21"/>
-      <c r="F124" s="21"/>
+      <c r="F124" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G124" s="22">
         <v>2</v>
       </c>
@@ -5249,7 +5452,9 @@
         <v>191</v>
       </c>
       <c r="E125" s="21"/>
-      <c r="F125" s="21"/>
+      <c r="F125" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G125" s="22">
         <v>4</v>
       </c>
@@ -5279,7 +5484,9 @@
         <v>193</v>
       </c>
       <c r="E126" s="21"/>
-      <c r="F126" s="21"/>
+      <c r="F126" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G126" s="22">
         <v>4</v>
       </c>
@@ -5309,7 +5516,9 @@
         <v>193</v>
       </c>
       <c r="E127" s="21"/>
-      <c r="F127" s="21"/>
+      <c r="F127" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G127" s="22">
         <v>2</v>
       </c>
@@ -5339,7 +5548,9 @@
         <v>194</v>
       </c>
       <c r="E128" s="21"/>
-      <c r="F128" s="21"/>
+      <c r="F128" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G128" s="22">
         <v>4</v>
       </c>
@@ -5369,7 +5580,9 @@
         <v>195</v>
       </c>
       <c r="E129" s="21"/>
-      <c r="F129" s="21"/>
+      <c r="F129" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G129" s="22">
         <v>2</v>
       </c>
@@ -5399,7 +5612,9 @@
         <v>191</v>
       </c>
       <c r="E130" s="21"/>
-      <c r="F130" s="21"/>
+      <c r="F130" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G130" s="22">
         <v>4</v>
       </c>
@@ -5429,7 +5644,9 @@
         <v>195</v>
       </c>
       <c r="E131" s="21"/>
-      <c r="F131" s="21"/>
+      <c r="F131" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G131" s="22">
         <v>2</v>
       </c>
@@ -5459,7 +5676,9 @@
         <v>191</v>
       </c>
       <c r="E132" s="21"/>
-      <c r="F132" s="21"/>
+      <c r="F132" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G132" s="22">
         <v>4</v>
       </c>
@@ -5489,7 +5708,9 @@
         <v>191</v>
       </c>
       <c r="E133" s="21"/>
-      <c r="F133" s="21"/>
+      <c r="F133" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G133" s="22">
         <v>3</v>
       </c>
@@ -5519,7 +5740,9 @@
         <v>195</v>
       </c>
       <c r="E134" s="21"/>
-      <c r="F134" s="21"/>
+      <c r="F134" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="G134" s="22">
         <v>2</v>
       </c>
@@ -5560,53 +5783,53 @@
       <c r="K135" s="31"/>
     </row>
     <row r="136" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A136" s="57" t="s">
+      <c r="A136" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="B136" s="58"/>
-      <c r="C136" s="58"/>
-      <c r="D136" s="58"/>
-      <c r="E136" s="58"/>
-      <c r="F136" s="58"/>
-      <c r="G136" s="58"/>
-      <c r="H136" s="58"/>
-      <c r="I136" s="58"/>
-      <c r="J136" s="58"/>
-      <c r="K136" s="59"/>
+      <c r="B136" s="66"/>
+      <c r="C136" s="66"/>
+      <c r="D136" s="66"/>
+      <c r="E136" s="66"/>
+      <c r="F136" s="66"/>
+      <c r="G136" s="66"/>
+      <c r="H136" s="66"/>
+      <c r="I136" s="66"/>
+      <c r="J136" s="66"/>
+      <c r="K136" s="67"/>
     </row>
     <row r="137" spans="1:11" ht="12.75">
       <c r="A137" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B137" s="60" t="s">
+      <c r="B137" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="C137" s="58"/>
-      <c r="D137" s="58"/>
-      <c r="E137" s="58"/>
-      <c r="F137" s="58"/>
-      <c r="G137" s="58"/>
-      <c r="H137" s="58"/>
-      <c r="I137" s="58"/>
-      <c r="J137" s="58"/>
-      <c r="K137" s="59"/>
+      <c r="C137" s="66"/>
+      <c r="D137" s="66"/>
+      <c r="E137" s="66"/>
+      <c r="F137" s="66"/>
+      <c r="G137" s="66"/>
+      <c r="H137" s="66"/>
+      <c r="I137" s="66"/>
+      <c r="J137" s="66"/>
+      <c r="K137" s="67"/>
     </row>
     <row r="138" spans="1:11" ht="28.5" customHeight="1">
       <c r="A138" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B138" s="60" t="s">
+      <c r="B138" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="C138" s="58"/>
-      <c r="D138" s="58"/>
-      <c r="E138" s="58"/>
-      <c r="F138" s="58"/>
-      <c r="G138" s="58"/>
-      <c r="H138" s="58"/>
-      <c r="I138" s="58"/>
-      <c r="J138" s="58"/>
-      <c r="K138" s="59"/>
+      <c r="C138" s="66"/>
+      <c r="D138" s="66"/>
+      <c r="E138" s="66"/>
+      <c r="F138" s="66"/>
+      <c r="G138" s="66"/>
+      <c r="H138" s="66"/>
+      <c r="I138" s="66"/>
+      <c r="J138" s="66"/>
+      <c r="K138" s="67"/>
     </row>
     <row r="139" spans="1:11" ht="12.75">
       <c r="A139" s="19">
@@ -5622,7 +5845,9 @@
         <v>209</v>
       </c>
       <c r="E139" s="21"/>
-      <c r="F139" s="21"/>
+      <c r="F139" s="21" t="s">
+        <v>228</v>
+      </c>
       <c r="G139" s="22">
         <v>3</v>
       </c>
@@ -5652,7 +5877,9 @@
         <v>210</v>
       </c>
       <c r="E140" s="21"/>
-      <c r="F140" s="21"/>
+      <c r="F140" s="21" t="s">
+        <v>228</v>
+      </c>
       <c r="G140" s="22">
         <v>2.5</v>
       </c>
@@ -5682,7 +5909,9 @@
         <v>211</v>
       </c>
       <c r="E141" s="21"/>
-      <c r="F141" s="21"/>
+      <c r="F141" s="21" t="s">
+        <v>228</v>
+      </c>
       <c r="G141" s="22">
         <v>3</v>
       </c>
@@ -5712,7 +5941,9 @@
         <v>212</v>
       </c>
       <c r="E142" s="21"/>
-      <c r="F142" s="21"/>
+      <c r="F142" s="21" t="s">
+        <v>228</v>
+      </c>
       <c r="G142" s="22">
         <v>1.5</v>
       </c>
@@ -5742,7 +5973,9 @@
         <v>213</v>
       </c>
       <c r="E143" s="21"/>
-      <c r="F143" s="21"/>
+      <c r="F143" s="21" t="s">
+        <v>228</v>
+      </c>
       <c r="G143" s="22">
         <v>4</v>
       </c>
@@ -5772,7 +6005,9 @@
         <v>70</v>
       </c>
       <c r="E144" s="21"/>
-      <c r="F144" s="21"/>
+      <c r="F144" s="21" t="s">
+        <v>228</v>
+      </c>
       <c r="G144" s="22">
         <v>1</v>
       </c>
@@ -5802,7 +6037,9 @@
         <v>214</v>
       </c>
       <c r="E145" s="21"/>
-      <c r="F145" s="21"/>
+      <c r="F145" s="21" t="s">
+        <v>228</v>
+      </c>
       <c r="G145" s="22">
         <v>2</v>
       </c>
@@ -5832,7 +6069,9 @@
         <v>215</v>
       </c>
       <c r="E146" s="21"/>
-      <c r="F146" s="21"/>
+      <c r="F146" s="21" t="s">
+        <v>228</v>
+      </c>
       <c r="G146" s="22">
         <v>4</v>
       </c>
@@ -5862,7 +6101,9 @@
         <v>215</v>
       </c>
       <c r="E147" s="21"/>
-      <c r="F147" s="21"/>
+      <c r="F147" s="21" t="s">
+        <v>228</v>
+      </c>
       <c r="G147" s="22">
         <v>4</v>
       </c>
@@ -5907,7 +6148,7 @@
   <customSheetViews>
     <customSheetView guid="{8BAC9A6B-5D32-4E8D-967D-E17D357516F8}" filter="1" showAutoFilter="1">
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="A1:K15" xr:uid="{7E226DFD-1936-4A1E-8E5E-9AC8C470802B}">
+      <autoFilter ref="A1:K15" xr:uid="{B00C608A-A5C8-4346-8E99-440E8E620512}">
         <filterColumn colId="1">
           <filters blank="1">
             <filter val="- Weekplan item 1_x000a_- Weekplan item 2_x000a_- Weekplan item 3_x000a_- etc"/>
@@ -5918,14 +6159,6 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="24">
-    <mergeCell ref="B101:K101"/>
-    <mergeCell ref="B102:K102"/>
-    <mergeCell ref="A119:K119"/>
-    <mergeCell ref="B63:K63"/>
-    <mergeCell ref="A81:K81"/>
-    <mergeCell ref="B82:K82"/>
-    <mergeCell ref="B83:K83"/>
-    <mergeCell ref="A100:K100"/>
     <mergeCell ref="A136:K136"/>
     <mergeCell ref="B137:K137"/>
     <mergeCell ref="B138:K138"/>
@@ -5942,6 +6175,14 @@
     <mergeCell ref="B120:K120"/>
     <mergeCell ref="B121:K121"/>
     <mergeCell ref="B62:K62"/>
+    <mergeCell ref="B101:K101"/>
+    <mergeCell ref="B102:K102"/>
+    <mergeCell ref="A119:K119"/>
+    <mergeCell ref="B63:K63"/>
+    <mergeCell ref="A81:K81"/>
+    <mergeCell ref="B82:K82"/>
+    <mergeCell ref="B83:K83"/>
+    <mergeCell ref="A100:K100"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:B20 B23:B40 B45:B59 B64:B79 B84:B98 B103:B117 B122:B134 B139:B147">
     <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Unplanned">
@@ -5986,8 +6227,8 @@
       <formula>H5/G5&lt;=0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" sqref="F5:F20 F25:F40 F64:F79 F45:F59 F84:F98 F103:F117 F122:F134 F139:F147" xr:uid="{0FAB3063-668E-4727-8636-10D0A6594410}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="F122:F134 F5:F20 F45:F59 F64:F79 F84:F98 F103:F117 F25:F40 F139:F147" xr:uid="{0FAB3063-668E-4727-8636-10D0A6594410}">
       <formula1>"ILO 1.6, ILO 2.6, ILO 5.1, ILO 6.4, ILO 8.6, ILO 8.7, ILO 8.8"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5998,7 +6239,7 @@
   <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'Drop-downs'!$B$2:$B$16</xm:f>
@@ -7660,23 +7901,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="493b2529-5793-4df3-af31-f67ebd481d19" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E12F46851DF89498422FB40BC19B005" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4a94336a3a0c3317dfb61e320cb9323a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="493b2529-5793-4df3-af31-f67ebd481d19" xmlns:ns4="30eab5da-4870-42fd-8792-80f96131dd9b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="00b4c09866ac1e8b5b5219b5e40e168f" ns3:_="" ns4:_="">
     <xsd:import namespace="493b2529-5793-4df3-af31-f67ebd481d19"/>
@@ -7915,32 +8139,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{320CF63A-30C9-4A8C-8DF9-EA62B8EC1A62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="30eab5da-4870-42fd-8792-80f96131dd9b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="493b2529-5793-4df3-af31-f67ebd481d19"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67A64A65-7DA4-4AE1-9847-B817073E4705}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="493b2529-5793-4df3-af31-f67ebd481d19" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD77405C-1A62-4A84-BBF1-D6001D0B1750}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7957,4 +8173,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67A64A65-7DA4-4AE1-9847-B817073E4705}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{320CF63A-30C9-4A8C-8DF9-EA62B8EC1A62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="30eab5da-4870-42fd-8792-80f96131dd9b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="493b2529-5793-4df3-af31-f67ebd481d19"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>